<commit_message>
dados alterados na planilha
</commit_message>
<xml_diff>
--- a/Registro-de-atividades.xlsx
+++ b/Registro-de-atividades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="286">
   <si>
     <t>Registro de atividades</t>
   </si>
@@ -823,6 +823,60 @@
   </si>
   <si>
     <t>Retirando  equipamentos de cima da mesa que vai ser retirada</t>
+  </si>
+  <si>
+    <t>Movendo mesa para a sala dos alunos de medicina</t>
+  </si>
+  <si>
+    <t>Verificando microfones de teto e cameras das salas do debrif</t>
+  </si>
+  <si>
+    <t>verificando fonte queimada lab 2</t>
+  </si>
+  <si>
+    <t>clonando imagem windows 11 nós computadores do lab 1</t>
+  </si>
+  <si>
+    <t>Instalando som na palestra no nissa</t>
+  </si>
+  <si>
+    <t>busando microfone no nissa</t>
+  </si>
+  <si>
+    <t>Ligando sistema de som no debrifing</t>
+  </si>
+  <si>
+    <t>Suporte tecnico aos professores semana academica</t>
+  </si>
+  <si>
+    <t>instalando zabbix na maquina lab-01-11</t>
+  </si>
+  <si>
+    <t>Instalando computadpres na sala do proex</t>
+  </si>
+  <si>
+    <t>Pegando caixa de som para carretinha levar para o nissa</t>
+  </si>
+  <si>
+    <t>NISSA</t>
+  </si>
+  <si>
+    <t>Instalando webcan no consultorio de odontologia e deixando notebook</t>
+  </si>
+  <si>
+    <t>Auxiliando professoa a projetar aula</t>
+  </si>
+  <si>
+    <t>Instalando caixas de som em evento de odontologia</t>
+  </si>
+  <si>
+    <t>Suporte a professora Juliana a conectar o notbook ao projetor</t>
+  </si>
+  <si>
+    <t>Manutenção em impressora epslon 3250</t>
+  </si>
+  <si>
+    <t>Conversado para entender como o workchat esta funcionando</t>
   </si>
 </sst>
 </file>
@@ -1525,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:V1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="G281" sqref="G281"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7514,151 +7568,562 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="282" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D282" s="11"/>
-      <c r="E282" s="10"/>
-      <c r="F282" s="10"/>
-      <c r="G282" s="10"/>
-      <c r="H282" s="11"/>
-      <c r="I282" s="11"/>
-    </row>
-    <row r="283" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D283" s="11"/>
-      <c r="E283" s="10"/>
-      <c r="F283" s="10"/>
-      <c r="G283" s="10"/>
-      <c r="H283" s="11"/>
-      <c r="I283" s="11"/>
-    </row>
-    <row r="284" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D284" s="11"/>
-      <c r="E284" s="10"/>
-      <c r="F284" s="10"/>
-      <c r="G284" s="10"/>
-      <c r="H284" s="11"/>
-      <c r="I284" s="11"/>
-    </row>
-    <row r="285" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D285" s="11"/>
-      <c r="E285" s="10"/>
-      <c r="F285" s="10"/>
-      <c r="G285" s="10"/>
-      <c r="H285" s="11"/>
-      <c r="I285" s="11"/>
-    </row>
-    <row r="286" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D286" s="11"/>
-      <c r="E286" s="10"/>
-      <c r="F286" s="10"/>
-      <c r="G286" s="10"/>
-      <c r="H286" s="11"/>
-      <c r="I286" s="11"/>
-    </row>
-    <row r="287" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D287" s="11"/>
-      <c r="E287" s="10"/>
-      <c r="F287" s="10"/>
-      <c r="G287" s="10"/>
-      <c r="H287" s="11"/>
-      <c r="I287" s="11"/>
-    </row>
-    <row r="288" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D288" s="11"/>
-      <c r="E288" s="10"/>
-      <c r="F288" s="10"/>
-      <c r="G288" s="10"/>
-      <c r="H288" s="11"/>
-      <c r="I288" s="11"/>
-    </row>
-    <row r="289" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D289" s="11"/>
-      <c r="E289" s="10"/>
-      <c r="F289" s="10"/>
-      <c r="G289" s="10"/>
-      <c r="H289" s="11"/>
-      <c r="I289" s="11"/>
-    </row>
-    <row r="290" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D290" s="11"/>
-      <c r="E290" s="10"/>
-      <c r="F290" s="10"/>
-      <c r="G290" s="10"/>
-      <c r="H290" s="11"/>
-      <c r="I290" s="11"/>
-    </row>
-    <row r="291" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D291" s="11"/>
-      <c r="E291" s="10"/>
-      <c r="F291" s="10"/>
-      <c r="G291" s="10"/>
-      <c r="H291" s="11"/>
-      <c r="I291" s="11"/>
-    </row>
-    <row r="292" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D292" s="11"/>
-      <c r="E292" s="10"/>
-      <c r="F292" s="10"/>
-      <c r="G292" s="10"/>
-      <c r="H292" s="11"/>
-      <c r="I292" s="11"/>
-    </row>
-    <row r="293" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D293" s="11"/>
-      <c r="E293" s="10"/>
-      <c r="F293" s="10"/>
-      <c r="G293" s="10"/>
-      <c r="H293" s="11"/>
-      <c r="I293" s="11"/>
-    </row>
-    <row r="294" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D294" s="11"/>
-      <c r="E294" s="10"/>
-      <c r="F294" s="10"/>
-      <c r="G294" s="10"/>
-      <c r="H294" s="11"/>
-      <c r="I294" s="11"/>
-    </row>
-    <row r="295" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D295" s="11"/>
-      <c r="E295" s="10"/>
-      <c r="F295" s="10"/>
-      <c r="G295" s="10"/>
-      <c r="H295" s="11"/>
-      <c r="I295" s="11"/>
-    </row>
-    <row r="296" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D296" s="11"/>
-      <c r="E296" s="10"/>
-      <c r="F296" s="10"/>
-      <c r="G296" s="10"/>
-      <c r="H296" s="11"/>
-      <c r="I296" s="11"/>
-    </row>
-    <row r="297" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D297" s="11"/>
-      <c r="E297" s="10"/>
-      <c r="F297" s="10"/>
-      <c r="G297" s="10"/>
-      <c r="H297" s="11"/>
-      <c r="I297" s="11"/>
-    </row>
-    <row r="298" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D298" s="11"/>
-      <c r="E298" s="10"/>
-      <c r="F298" s="10"/>
-      <c r="G298" s="10"/>
-      <c r="H298" s="11"/>
-      <c r="I298" s="11"/>
-    </row>
-    <row r="299" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D299" s="11"/>
-      <c r="E299" s="10"/>
-      <c r="F299" s="10"/>
-      <c r="G299" s="10"/>
-      <c r="H299" s="11"/>
-      <c r="I299" s="11"/>
-    </row>
-    <row r="300" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D282" s="4">
+        <v>45604</v>
+      </c>
+      <c r="E282" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F282" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G282" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="H282" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="I282" s="6">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="283" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="22"/>
+      <c r="B283" s="22"/>
+      <c r="C283" s="23"/>
+      <c r="D283" s="24">
+        <v>45607</v>
+      </c>
+      <c r="E283" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F283" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G283" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H283" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I283" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="J283" s="22"/>
+      <c r="K283" s="22"/>
+      <c r="L283" s="22"/>
+      <c r="M283" s="22"/>
+      <c r="N283" s="22"/>
+      <c r="O283" s="22"/>
+    </row>
+    <row r="284" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="22"/>
+      <c r="B284" s="22"/>
+      <c r="C284" s="23"/>
+      <c r="D284" s="36">
+        <v>45607</v>
+      </c>
+      <c r="E284" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F284" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G284" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="H284" s="19">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I284" s="19">
+        <v>0.5625</v>
+      </c>
+      <c r="J284" s="22"/>
+      <c r="K284" s="22"/>
+      <c r="L284" s="22"/>
+      <c r="M284" s="22"/>
+      <c r="N284" s="22"/>
+      <c r="O284" s="22"/>
+    </row>
+    <row r="285" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="22"/>
+      <c r="B285" s="22"/>
+      <c r="C285" s="23"/>
+      <c r="D285" s="36">
+        <v>45608</v>
+      </c>
+      <c r="E285" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F285" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G285" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="H285" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I285" s="19">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J285" s="22"/>
+      <c r="K285" s="22"/>
+      <c r="L285" s="22"/>
+      <c r="M285" s="22"/>
+      <c r="N285" s="22"/>
+      <c r="O285" s="22"/>
+    </row>
+    <row r="286" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="22"/>
+      <c r="B286" s="22"/>
+      <c r="C286" s="23"/>
+      <c r="D286" s="36">
+        <v>45609</v>
+      </c>
+      <c r="E286" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F286" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G286" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="H286" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I286" s="19">
+        <v>0.375</v>
+      </c>
+      <c r="J286" s="22"/>
+      <c r="K286" s="22"/>
+      <c r="L286" s="22"/>
+      <c r="M286" s="22"/>
+      <c r="N286" s="22"/>
+      <c r="O286" s="22"/>
+    </row>
+    <row r="287" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="22"/>
+      <c r="B287" s="22"/>
+      <c r="C287" s="23"/>
+      <c r="D287" s="36">
+        <v>45609</v>
+      </c>
+      <c r="E287" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F287" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G287" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="H287" s="19">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="I287" s="19">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J287" s="22"/>
+      <c r="K287" s="22"/>
+      <c r="L287" s="22"/>
+      <c r="M287" s="22"/>
+      <c r="N287" s="22"/>
+      <c r="O287" s="22"/>
+    </row>
+    <row r="288" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="22"/>
+      <c r="B288" s="22"/>
+      <c r="C288" s="23"/>
+      <c r="D288" s="36">
+        <v>45609</v>
+      </c>
+      <c r="E288" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F288" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G288" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H288" s="19">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I288" s="19">
+        <v>0.54652777777777783</v>
+      </c>
+      <c r="J288" s="22"/>
+      <c r="K288" s="22"/>
+      <c r="L288" s="22"/>
+      <c r="M288" s="22"/>
+      <c r="N288" s="22"/>
+      <c r="O288" s="22"/>
+    </row>
+    <row r="289" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="22"/>
+      <c r="B289" s="22"/>
+      <c r="C289" s="23"/>
+      <c r="D289" s="36">
+        <v>45609</v>
+      </c>
+      <c r="E289" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F289" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G289" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="H289" s="19">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="I289" s="19">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J289" s="22"/>
+      <c r="K289" s="22"/>
+      <c r="L289" s="22"/>
+      <c r="M289" s="22"/>
+      <c r="N289" s="22"/>
+      <c r="O289" s="22"/>
+    </row>
+    <row r="290" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="22"/>
+      <c r="B290" s="22"/>
+      <c r="C290" s="23"/>
+      <c r="D290" s="36">
+        <v>45610</v>
+      </c>
+      <c r="E290" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F290" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G290" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="H290" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I290" s="19">
+        <v>0.375</v>
+      </c>
+      <c r="J290" s="22"/>
+      <c r="K290" s="22"/>
+      <c r="L290" s="22"/>
+      <c r="M290" s="22"/>
+      <c r="N290" s="22"/>
+      <c r="O290" s="22"/>
+    </row>
+    <row r="291" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="22"/>
+      <c r="B291" s="22"/>
+      <c r="C291" s="23"/>
+      <c r="D291" s="36">
+        <v>45610</v>
+      </c>
+      <c r="E291" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F291" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G291" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="H291" s="19">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="I291" s="19">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="J291" s="22"/>
+      <c r="K291" s="22"/>
+      <c r="L291" s="22"/>
+      <c r="M291" s="22"/>
+      <c r="N291" s="22"/>
+      <c r="O291" s="22"/>
+    </row>
+    <row r="292" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="22"/>
+      <c r="B292" s="22"/>
+      <c r="C292" s="23"/>
+      <c r="D292" s="36">
+        <v>45610</v>
+      </c>
+      <c r="E292" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F292" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G292" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="H292" s="19">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="I292" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J292" s="22"/>
+      <c r="K292" s="22"/>
+      <c r="L292" s="22"/>
+      <c r="M292" s="22"/>
+      <c r="N292" s="22"/>
+      <c r="O292" s="22"/>
+    </row>
+    <row r="293" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="22"/>
+      <c r="B293" s="22"/>
+      <c r="C293" s="23"/>
+      <c r="D293" s="36">
+        <v>45610</v>
+      </c>
+      <c r="E293" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F293" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G293" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="H293" s="19">
+        <v>0.39652777777777781</v>
+      </c>
+      <c r="I293" s="19">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="J293" s="22"/>
+      <c r="K293" s="22"/>
+      <c r="L293" s="22"/>
+      <c r="M293" s="22"/>
+      <c r="N293" s="22"/>
+      <c r="O293" s="22"/>
+    </row>
+    <row r="294" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="22"/>
+      <c r="B294" s="22"/>
+      <c r="C294" s="23"/>
+      <c r="D294" s="24">
+        <v>45610</v>
+      </c>
+      <c r="E294" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F294" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G294" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H294" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="I294" s="16">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="J294" s="22"/>
+      <c r="K294" s="22"/>
+      <c r="L294" s="22"/>
+      <c r="M294" s="22"/>
+      <c r="N294" s="22"/>
+      <c r="O294" s="22"/>
+      <c r="P294" s="22"/>
+      <c r="Q294" s="22"/>
+      <c r="R294" s="22"/>
+      <c r="S294" s="22"/>
+      <c r="T294" s="22"/>
+      <c r="U294" s="22"/>
+      <c r="V294" s="22"/>
+    </row>
+    <row r="295" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="22"/>
+      <c r="B295" s="22"/>
+      <c r="C295" s="23"/>
+      <c r="D295" s="36">
+        <v>45610</v>
+      </c>
+      <c r="E295" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F295" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G295" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="H295" s="19">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="I295" s="19">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="J295" s="22"/>
+      <c r="K295" s="22"/>
+      <c r="L295" s="22"/>
+      <c r="M295" s="22"/>
+      <c r="N295" s="22"/>
+      <c r="O295" s="22"/>
+      <c r="P295" s="22"/>
+      <c r="Q295" s="22"/>
+      <c r="R295" s="22"/>
+      <c r="S295" s="22"/>
+      <c r="T295" s="22"/>
+      <c r="U295" s="22"/>
+      <c r="V295" s="22"/>
+    </row>
+    <row r="296" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="22"/>
+      <c r="B296" s="22"/>
+      <c r="C296" s="23"/>
+      <c r="D296" s="24">
+        <v>45610</v>
+      </c>
+      <c r="E296" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F296" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G296" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="H296" s="16">
+        <v>0.5625</v>
+      </c>
+      <c r="I296" s="16">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="J296" s="22"/>
+      <c r="K296" s="22"/>
+      <c r="L296" s="22"/>
+      <c r="M296" s="22"/>
+      <c r="N296" s="22"/>
+      <c r="O296" s="22"/>
+      <c r="P296" s="22"/>
+      <c r="Q296" s="22"/>
+      <c r="R296" s="22"/>
+      <c r="S296" s="22"/>
+      <c r="T296" s="22"/>
+      <c r="U296" s="22"/>
+      <c r="V296" s="22"/>
+    </row>
+    <row r="297" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="22"/>
+      <c r="B297" s="22"/>
+      <c r="C297" s="23"/>
+      <c r="D297" s="36">
+        <v>45614</v>
+      </c>
+      <c r="E297" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F297" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G297" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="H297" s="19">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="I297" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="J297" s="22"/>
+      <c r="K297" s="22"/>
+      <c r="L297" s="22"/>
+      <c r="M297" s="22"/>
+      <c r="N297" s="22"/>
+      <c r="O297" s="22"/>
+      <c r="P297" s="22"/>
+      <c r="Q297" s="22"/>
+      <c r="R297" s="22"/>
+      <c r="S297" s="22"/>
+      <c r="T297" s="22"/>
+      <c r="U297" s="22"/>
+      <c r="V297" s="22"/>
+    </row>
+    <row r="298" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="22"/>
+      <c r="B298" s="22"/>
+      <c r="C298" s="23"/>
+      <c r="D298" s="24">
+        <v>45614</v>
+      </c>
+      <c r="E298" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F298" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="G298" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="H298" s="16">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="I298" s="16">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="J298" s="22"/>
+      <c r="K298" s="22"/>
+      <c r="L298" s="22"/>
+      <c r="M298" s="22"/>
+      <c r="N298" s="22"/>
+      <c r="O298" s="22"/>
+      <c r="P298" s="22"/>
+      <c r="Q298" s="22"/>
+      <c r="R298" s="22"/>
+      <c r="S298" s="22"/>
+      <c r="T298" s="22"/>
+      <c r="U298" s="22"/>
+      <c r="V298" s="22"/>
+    </row>
+    <row r="299" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="22"/>
+      <c r="B299" s="22"/>
+      <c r="C299" s="23"/>
+      <c r="D299" s="24">
+        <v>45614</v>
+      </c>
+      <c r="E299" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F299" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G299" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="H299" s="16">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="I299" s="16">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="J299" s="22"/>
+      <c r="K299" s="22"/>
+      <c r="L299" s="22"/>
+      <c r="M299" s="22"/>
+      <c r="N299" s="22"/>
+      <c r="O299" s="22"/>
+      <c r="P299" s="22"/>
+      <c r="Q299" s="22"/>
+      <c r="R299" s="22"/>
+      <c r="S299" s="22"/>
+      <c r="T299" s="22"/>
+      <c r="U299" s="22"/>
+      <c r="V299" s="22"/>
+    </row>
+    <row r="300" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D300" s="11"/>
       <c r="E300" s="10"/>
       <c r="F300" s="10"/>
@@ -7666,7 +8131,7 @@
       <c r="H300" s="11"/>
       <c r="I300" s="11"/>
     </row>
-    <row r="301" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D301" s="11"/>
       <c r="E301" s="10"/>
       <c r="F301" s="10"/>
@@ -7674,7 +8139,7 @@
       <c r="H301" s="11"/>
       <c r="I301" s="11"/>
     </row>
-    <row r="302" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D302" s="11"/>
       <c r="E302" s="10"/>
       <c r="F302" s="10"/>
@@ -7682,7 +8147,7 @@
       <c r="H302" s="11"/>
       <c r="I302" s="11"/>
     </row>
-    <row r="303" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D303" s="11"/>
       <c r="E303" s="10"/>
       <c r="F303" s="10"/>
@@ -7690,7 +8155,7 @@
       <c r="H303" s="11"/>
       <c r="I303" s="11"/>
     </row>
-    <row r="304" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D304" s="11"/>
       <c r="E304" s="10"/>
       <c r="F304" s="10"/>
@@ -13336,13 +13801,13 @@
     <mergeCell ref="C1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E1008">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E282 E300:E1008">
       <formula1>"GABRIEL,UILLIAM"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F32 F40">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F1008">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F282 F300:F1008">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CPA,CORD,BLIB,DIR,FIN,RH"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F28">

</xml_diff>

<commit_message>
novos dados na planilha
</commit_message>
<xml_diff>
--- a/Registro-de-atividades.xlsx
+++ b/Registro-de-atividades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="335">
   <si>
     <t>Registro de atividades</t>
   </si>
@@ -877,6 +877,153 @@
   </si>
   <si>
     <t>Conversado para entender como o workchat esta funcionando</t>
+  </si>
+  <si>
+    <t>Guardando notebooks</t>
+  </si>
+  <si>
+    <t>Regeistrando nomes e telefones na planilha leads ENEM 2024.2</t>
+  </si>
+  <si>
+    <t>Fazenedo testes nos pcs do lab 01</t>
+  </si>
+  <si>
+    <t>Formatando pc lab 01</t>
+  </si>
+  <si>
+    <t>Acompanhando João no treinamento dp work chat</t>
+  </si>
+  <si>
+    <t>recolhendo equipamentos do ti na clinica de odonto</t>
+  </si>
+  <si>
+    <t>Instalando pc lab-01-20 no laboratorio</t>
+  </si>
+  <si>
+    <t>Suporte na projeção e conexão ao som</t>
+  </si>
+  <si>
+    <t>Levando impressora hd para a informak</t>
+  </si>
+  <si>
+    <t>tentando resolver bug do rotaFacenp</t>
+  </si>
+  <si>
+    <t>Refazendo estenção que estava dando curto</t>
+  </si>
+  <si>
+    <t>Tirando fios do debrif</t>
+  </si>
+  <si>
+    <t>Indentificando cabos de som e cortando gesso das salas do debri 2 e 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passando cabos nas salas do debrif </t>
+  </si>
+  <si>
+    <t>Acompanhando na fechamento do gesso na sala do debrif</t>
+  </si>
+  <si>
+    <t>Importando dados para o CRM</t>
+  </si>
+  <si>
+    <t>Tracando teclado do computador de Rita</t>
+  </si>
+  <si>
+    <t>Ligando Equipamentos de medicina</t>
+  </si>
+  <si>
+    <t>Gravando video para rita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizando acompanhamento a gravação de comercial </t>
+  </si>
+  <si>
+    <t>Realizando manutenção pc da sala de metodolgias ativas</t>
+  </si>
+  <si>
+    <t>Guardando cabos no deposito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consertando extenções </t>
+  </si>
+  <si>
+    <t>Consertando impressora da secretaria</t>
+  </si>
+  <si>
+    <t>Suporte a João no curso de treinamento a mexer nos bonecos de medicina</t>
+  </si>
+  <si>
+    <t>Importando arquivos para o RD Station CRM</t>
+  </si>
+  <si>
+    <t>Fazendo teste no computador da sala de metodologias ativas</t>
+  </si>
+  <si>
+    <t>cabos fixados na mesa de controle do Debrifing 1, 2 e 3</t>
+  </si>
+  <si>
+    <t>Fixando os 8 computadores e monitores, instalar computadores nas salas de aula</t>
+  </si>
+  <si>
+    <t>Ligando as televisões</t>
+  </si>
+  <si>
+    <t>Fixando os cabos dos computadores da secretaria após a mudança de mesas</t>
+  </si>
+  <si>
+    <t>Fixando cabos na captação, organizar cabos e filtro de linha</t>
+  </si>
+  <si>
+    <t>Fixando fios da speed dome na sala de habilidades clínicas</t>
+  </si>
+  <si>
+    <t>Colocando computador login na sala de apoio tecnico</t>
+  </si>
+  <si>
+    <t>Guardando notbook</t>
+  </si>
+  <si>
+    <t>Instalando e configurando impressora</t>
+  </si>
+  <si>
+    <t>Configurando sistema de buscar sala no linux</t>
+  </si>
+  <si>
+    <t>guardando notbook</t>
+  </si>
+  <si>
+    <t>Ligando televisoões</t>
+  </si>
+  <si>
+    <t>importando videos do app mapa de sala</t>
+  </si>
+  <si>
+    <t>levando microtic lem Fernando</t>
+  </si>
+  <si>
+    <t>editando videos do app mapa de sala</t>
+  </si>
+  <si>
+    <t>Ligando equipamentos no debrif</t>
+  </si>
+  <si>
+    <t>Tirando entrada de ar da impressora epson</t>
+  </si>
+  <si>
+    <t>Ligando monitor</t>
+  </si>
+  <si>
+    <t>realizando orçamento de equipamentos de som</t>
+  </si>
+  <si>
+    <t>programando mapa de sala</t>
+  </si>
+  <si>
+    <t>Instalando TOTVS na computador de dona Leonor</t>
+  </si>
+  <si>
+    <t>instalando DVR</t>
   </si>
 </sst>
 </file>
@@ -886,7 +1033,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -953,6 +1100,13 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1218,7 +1372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1350,6 +1504,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1577,10 +1755,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1008"/>
+  <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="C300" sqref="C300"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="A353" sqref="A353:X356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1592,17 +1770,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="53" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -8123,463 +8301,1803 @@
       <c r="U299" s="22"/>
       <c r="V299" s="22"/>
     </row>
-    <row r="300" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D300" s="11"/>
-      <c r="E300" s="10"/>
-      <c r="F300" s="10"/>
-      <c r="G300" s="10"/>
-      <c r="H300" s="11"/>
-      <c r="I300" s="11"/>
-    </row>
-    <row r="301" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D301" s="11"/>
-      <c r="E301" s="10"/>
-      <c r="F301" s="10"/>
-      <c r="G301" s="10"/>
-      <c r="H301" s="11"/>
-      <c r="I301" s="11"/>
-    </row>
-    <row r="302" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D302" s="11"/>
-      <c r="E302" s="10"/>
-      <c r="F302" s="10"/>
-      <c r="G302" s="10"/>
-      <c r="H302" s="11"/>
-      <c r="I302" s="11"/>
+    <row r="300" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D300" s="4">
+        <v>45615</v>
+      </c>
+      <c r="E300" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F300" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G300" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H300" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I300" s="6">
+        <v>0.33680555555555558</v>
+      </c>
+    </row>
+    <row r="301" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="22"/>
+      <c r="B301" s="22"/>
+      <c r="C301" s="23"/>
+      <c r="D301" s="24">
+        <v>45615</v>
+      </c>
+      <c r="E301" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F301" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G301" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="H301" s="16">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I301" s="16">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="J301" s="22"/>
+      <c r="K301" s="22"/>
+      <c r="L301" s="22"/>
+      <c r="M301" s="22"/>
+      <c r="N301" s="22"/>
+      <c r="O301" s="22"/>
+      <c r="P301" s="22"/>
+      <c r="Q301" s="22"/>
+      <c r="R301" s="22"/>
+      <c r="S301" s="22"/>
+      <c r="T301" s="22"/>
+      <c r="U301" s="22"/>
+      <c r="V301" s="22"/>
+    </row>
+    <row r="302" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="22"/>
+      <c r="B302" s="22"/>
+      <c r="C302" s="23"/>
+      <c r="D302" s="36">
+        <v>45615</v>
+      </c>
+      <c r="E302" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F302" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G302" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H302" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I302" s="19">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="J302" s="22"/>
+      <c r="K302" s="22"/>
+      <c r="L302" s="22"/>
+      <c r="M302" s="22"/>
+      <c r="N302" s="22"/>
+      <c r="O302" s="22"/>
+      <c r="P302" s="22"/>
+      <c r="Q302" s="22"/>
+      <c r="R302" s="22"/>
+      <c r="S302" s="22"/>
+      <c r="T302" s="22"/>
+      <c r="U302" s="22"/>
+      <c r="V302" s="22"/>
     </row>
     <row r="303" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D303" s="11"/>
-      <c r="E303" s="10"/>
-      <c r="F303" s="10"/>
-      <c r="G303" s="10"/>
-      <c r="H303" s="11"/>
-      <c r="I303" s="11"/>
-    </row>
-    <row r="304" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D304" s="11"/>
-      <c r="E304" s="10"/>
-      <c r="F304" s="10"/>
-      <c r="G304" s="10"/>
-      <c r="H304" s="11"/>
-      <c r="I304" s="11"/>
-    </row>
-    <row r="305" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D305" s="11"/>
-      <c r="E305" s="10"/>
-      <c r="F305" s="10"/>
-      <c r="G305" s="10"/>
-      <c r="H305" s="11"/>
-      <c r="I305" s="11"/>
-    </row>
-    <row r="306" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D306" s="11"/>
-      <c r="E306" s="10"/>
-      <c r="F306" s="10"/>
-      <c r="G306" s="10"/>
-      <c r="H306" s="11"/>
-      <c r="I306" s="11"/>
-    </row>
-    <row r="307" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D307" s="11"/>
-      <c r="E307" s="10"/>
-      <c r="F307" s="10"/>
-      <c r="G307" s="10"/>
-      <c r="H307" s="11"/>
-      <c r="I307" s="11"/>
-    </row>
-    <row r="308" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D308" s="11"/>
-      <c r="E308" s="10"/>
-      <c r="F308" s="10"/>
-      <c r="G308" s="10"/>
-      <c r="H308" s="11"/>
-      <c r="I308" s="11"/>
-    </row>
-    <row r="309" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D309" s="11"/>
-      <c r="E309" s="10"/>
-      <c r="F309" s="10"/>
-      <c r="G309" s="10"/>
-      <c r="H309" s="11"/>
-      <c r="I309" s="11"/>
-    </row>
-    <row r="310" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D310" s="11"/>
-      <c r="E310" s="10"/>
-      <c r="F310" s="10"/>
-      <c r="G310" s="10"/>
-      <c r="H310" s="11"/>
-      <c r="I310" s="11"/>
-    </row>
-    <row r="311" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D311" s="11"/>
-      <c r="E311" s="10"/>
-      <c r="F311" s="10"/>
-      <c r="G311" s="10"/>
-      <c r="H311" s="11"/>
-      <c r="I311" s="11"/>
-    </row>
-    <row r="312" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D312" s="11"/>
-      <c r="E312" s="10"/>
-      <c r="F312" s="10"/>
-      <c r="G312" s="10"/>
-      <c r="H312" s="11"/>
-      <c r="I312" s="11"/>
-    </row>
-    <row r="313" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D313" s="11"/>
-      <c r="E313" s="10"/>
-      <c r="F313" s="10"/>
-      <c r="G313" s="10"/>
-      <c r="H313" s="11"/>
-      <c r="I313" s="11"/>
-    </row>
-    <row r="314" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D314" s="11"/>
-      <c r="E314" s="10"/>
-      <c r="F314" s="10"/>
-      <c r="G314" s="10"/>
-      <c r="H314" s="11"/>
-      <c r="I314" s="11"/>
-    </row>
-    <row r="315" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D315" s="11"/>
-      <c r="E315" s="10"/>
-      <c r="F315" s="10"/>
-      <c r="G315" s="10"/>
-      <c r="H315" s="11"/>
-      <c r="I315" s="11"/>
-    </row>
-    <row r="316" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D316" s="11"/>
-      <c r="E316" s="10"/>
-      <c r="F316" s="10"/>
-      <c r="G316" s="10"/>
-      <c r="H316" s="11"/>
-      <c r="I316" s="11"/>
-    </row>
-    <row r="317" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D317" s="11"/>
-      <c r="E317" s="10"/>
-      <c r="F317" s="10"/>
-      <c r="G317" s="10"/>
-      <c r="H317" s="11"/>
-      <c r="I317" s="11"/>
-    </row>
-    <row r="318" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D318" s="11"/>
-      <c r="E318" s="10"/>
-      <c r="F318" s="10"/>
-      <c r="G318" s="10"/>
-      <c r="H318" s="11"/>
-      <c r="I318" s="11"/>
-    </row>
-    <row r="319" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D319" s="11"/>
-      <c r="E319" s="10"/>
-      <c r="F319" s="10"/>
-      <c r="G319" s="10"/>
-      <c r="H319" s="11"/>
-      <c r="I319" s="11"/>
-    </row>
-    <row r="320" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D320" s="11"/>
-      <c r="E320" s="10"/>
-      <c r="F320" s="10"/>
-      <c r="G320" s="10"/>
-      <c r="H320" s="11"/>
-      <c r="I320" s="11"/>
-    </row>
-    <row r="321" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D321" s="11"/>
-      <c r="E321" s="10"/>
-      <c r="F321" s="10"/>
-      <c r="G321" s="10"/>
-      <c r="H321" s="11"/>
-      <c r="I321" s="11"/>
-    </row>
-    <row r="322" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D322" s="11"/>
-      <c r="E322" s="10"/>
-      <c r="F322" s="10"/>
-      <c r="G322" s="10"/>
-      <c r="H322" s="11"/>
-      <c r="I322" s="11"/>
-    </row>
-    <row r="323" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D323" s="11"/>
-      <c r="E323" s="10"/>
-      <c r="F323" s="10"/>
-      <c r="G323" s="10"/>
-      <c r="H323" s="11"/>
-      <c r="I323" s="11"/>
-    </row>
-    <row r="324" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D324" s="11"/>
-      <c r="E324" s="10"/>
-      <c r="F324" s="10"/>
-      <c r="G324" s="10"/>
-      <c r="H324" s="11"/>
-      <c r="I324" s="11"/>
-    </row>
-    <row r="325" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D325" s="11"/>
-      <c r="E325" s="10"/>
-      <c r="F325" s="10"/>
-      <c r="G325" s="10"/>
-      <c r="H325" s="11"/>
-      <c r="I325" s="11"/>
-    </row>
-    <row r="326" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D326" s="11"/>
-      <c r="E326" s="10"/>
-      <c r="F326" s="10"/>
-      <c r="G326" s="10"/>
-      <c r="H326" s="11"/>
-      <c r="I326" s="11"/>
-    </row>
-    <row r="327" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D327" s="11"/>
-      <c r="E327" s="10"/>
-      <c r="F327" s="10"/>
-      <c r="G327" s="10"/>
-      <c r="H327" s="11"/>
-      <c r="I327" s="11"/>
-    </row>
-    <row r="328" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D328" s="11"/>
-      <c r="E328" s="10"/>
-      <c r="F328" s="10"/>
-      <c r="G328" s="10"/>
-      <c r="H328" s="11"/>
-      <c r="I328" s="11"/>
-    </row>
-    <row r="329" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D329" s="11"/>
-      <c r="E329" s="10"/>
-      <c r="F329" s="10"/>
-      <c r="G329" s="10"/>
-      <c r="H329" s="11"/>
-      <c r="I329" s="11"/>
-    </row>
-    <row r="330" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D330" s="11"/>
-      <c r="E330" s="10"/>
-      <c r="F330" s="10"/>
-      <c r="G330" s="10"/>
-      <c r="H330" s="11"/>
-      <c r="I330" s="11"/>
-    </row>
-    <row r="331" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D331" s="11"/>
-      <c r="E331" s="10"/>
-      <c r="F331" s="10"/>
-      <c r="G331" s="10"/>
-      <c r="H331" s="11"/>
-      <c r="I331" s="11"/>
-    </row>
-    <row r="332" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D332" s="11"/>
-      <c r="E332" s="10"/>
-      <c r="F332" s="10"/>
-      <c r="G332" s="10"/>
-      <c r="H332" s="11"/>
-      <c r="I332" s="11"/>
-    </row>
-    <row r="333" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D333" s="11"/>
-      <c r="E333" s="10"/>
-      <c r="F333" s="10"/>
-      <c r="G333" s="10"/>
-      <c r="H333" s="11"/>
-      <c r="I333" s="11"/>
-    </row>
-    <row r="334" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D334" s="11"/>
-      <c r="E334" s="10"/>
-      <c r="F334" s="10"/>
-      <c r="G334" s="10"/>
-      <c r="H334" s="11"/>
-      <c r="I334" s="11"/>
-    </row>
-    <row r="335" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D335" s="11"/>
-      <c r="E335" s="10"/>
-      <c r="F335" s="10"/>
-      <c r="G335" s="10"/>
-      <c r="H335" s="11"/>
-      <c r="I335" s="11"/>
-    </row>
-    <row r="336" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D336" s="11"/>
-      <c r="E336" s="10"/>
-      <c r="F336" s="10"/>
-      <c r="G336" s="10"/>
-      <c r="H336" s="11"/>
-      <c r="I336" s="11"/>
-    </row>
-    <row r="337" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D337" s="11"/>
-      <c r="E337" s="10"/>
-      <c r="F337" s="10"/>
-      <c r="G337" s="10"/>
-      <c r="H337" s="11"/>
-      <c r="I337" s="11"/>
-    </row>
-    <row r="338" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D338" s="11"/>
-      <c r="E338" s="10"/>
-      <c r="F338" s="10"/>
-      <c r="G338" s="10"/>
-      <c r="H338" s="11"/>
-      <c r="I338" s="11"/>
-    </row>
-    <row r="339" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D339" s="11"/>
-      <c r="E339" s="10"/>
-      <c r="F339" s="10"/>
-      <c r="G339" s="10"/>
-      <c r="H339" s="11"/>
-      <c r="I339" s="11"/>
-    </row>
-    <row r="340" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D340" s="11"/>
-      <c r="E340" s="10"/>
-      <c r="F340" s="10"/>
-      <c r="G340" s="10"/>
-      <c r="H340" s="11"/>
-      <c r="I340" s="11"/>
-    </row>
-    <row r="341" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D341" s="11"/>
-      <c r="E341" s="10"/>
-      <c r="F341" s="10"/>
-      <c r="G341" s="10"/>
-      <c r="H341" s="11"/>
-      <c r="I341" s="11"/>
-    </row>
-    <row r="342" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D342" s="11"/>
-      <c r="E342" s="10"/>
-      <c r="F342" s="10"/>
-      <c r="G342" s="10"/>
-      <c r="H342" s="11"/>
-      <c r="I342" s="11"/>
-    </row>
-    <row r="343" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D343" s="11"/>
-      <c r="E343" s="10"/>
-      <c r="F343" s="10"/>
-      <c r="G343" s="10"/>
-      <c r="H343" s="11"/>
-      <c r="I343" s="11"/>
-    </row>
-    <row r="344" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D344" s="11"/>
-      <c r="E344" s="10"/>
-      <c r="F344" s="10"/>
-      <c r="G344" s="10"/>
-      <c r="H344" s="11"/>
-      <c r="I344" s="11"/>
-    </row>
-    <row r="345" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D345" s="11"/>
-      <c r="E345" s="10"/>
-      <c r="F345" s="10"/>
-      <c r="G345" s="10"/>
-      <c r="H345" s="11"/>
-      <c r="I345" s="11"/>
-    </row>
-    <row r="346" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D346" s="11"/>
-      <c r="E346" s="10"/>
-      <c r="F346" s="10"/>
-      <c r="G346" s="10"/>
-      <c r="H346" s="11"/>
-      <c r="I346" s="11"/>
-    </row>
-    <row r="347" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D347" s="11"/>
-      <c r="E347" s="10"/>
-      <c r="F347" s="10"/>
-      <c r="G347" s="10"/>
-      <c r="H347" s="11"/>
-      <c r="I347" s="11"/>
-    </row>
-    <row r="348" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D348" s="11"/>
-      <c r="E348" s="10"/>
-      <c r="F348" s="10"/>
-      <c r="G348" s="10"/>
-      <c r="H348" s="11"/>
-      <c r="I348" s="11"/>
-    </row>
-    <row r="349" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D349" s="11"/>
-      <c r="E349" s="10"/>
-      <c r="F349" s="10"/>
-      <c r="G349" s="10"/>
-      <c r="H349" s="11"/>
-      <c r="I349" s="11"/>
-    </row>
-    <row r="350" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D350" s="11"/>
-      <c r="E350" s="10"/>
-      <c r="F350" s="10"/>
-      <c r="G350" s="10"/>
-      <c r="H350" s="11"/>
-      <c r="I350" s="11"/>
-    </row>
-    <row r="351" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D351" s="11"/>
-      <c r="E351" s="10"/>
-      <c r="F351" s="10"/>
-      <c r="G351" s="10"/>
-      <c r="H351" s="11"/>
-      <c r="I351" s="11"/>
-    </row>
-    <row r="352" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D352" s="11"/>
-      <c r="E352" s="10"/>
-      <c r="F352" s="10"/>
-      <c r="G352" s="10"/>
-      <c r="H352" s="11"/>
-      <c r="I352" s="11"/>
-    </row>
-    <row r="353" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D353" s="11"/>
-      <c r="E353" s="10"/>
-      <c r="F353" s="10"/>
-      <c r="G353" s="10"/>
-      <c r="H353" s="11"/>
-      <c r="I353" s="11"/>
-    </row>
-    <row r="354" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D354" s="11"/>
-      <c r="E354" s="10"/>
-      <c r="F354" s="10"/>
-      <c r="G354" s="10"/>
-      <c r="H354" s="11"/>
-      <c r="I354" s="11"/>
-    </row>
-    <row r="355" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D355" s="11"/>
-      <c r="E355" s="10"/>
-      <c r="F355" s="10"/>
-      <c r="G355" s="10"/>
-      <c r="H355" s="11"/>
-      <c r="I355" s="11"/>
-    </row>
-    <row r="356" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D356" s="11"/>
-      <c r="E356" s="10"/>
-      <c r="F356" s="10"/>
-      <c r="G356" s="10"/>
-      <c r="H356" s="11"/>
-      <c r="I356" s="11"/>
-    </row>
-    <row r="357" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D303" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E303" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F303" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G303" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="H303" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I303" s="6">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="304" spans="1:22" s="51" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D304" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E304" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F304" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G304" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H304" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I304" s="6">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="305" spans="1:23" s="51" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D305" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E305" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F305" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G305" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H305" s="6">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="I305" s="6">
+        <v>0.4055555555555555</v>
+      </c>
+    </row>
+    <row r="306" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D306" s="4">
+        <v>45617</v>
+      </c>
+      <c r="E306" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F306" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G306" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H306" s="6">
+        <v>0.40625</v>
+      </c>
+      <c r="I306" s="6">
+        <v>0.4201388888888889</v>
+      </c>
+    </row>
+    <row r="307" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="22"/>
+      <c r="B307" s="22"/>
+      <c r="C307" s="23"/>
+      <c r="D307" s="24">
+        <v>45617</v>
+      </c>
+      <c r="E307" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F307" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G307" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="H307" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I307" s="16">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="J307" s="22"/>
+      <c r="K307" s="22"/>
+      <c r="L307" s="22"/>
+      <c r="M307" s="22"/>
+      <c r="N307" s="22"/>
+      <c r="O307" s="22"/>
+      <c r="P307" s="22"/>
+      <c r="Q307" s="22"/>
+      <c r="R307" s="22"/>
+      <c r="S307" s="22"/>
+      <c r="T307" s="22"/>
+      <c r="U307" s="22"/>
+      <c r="V307" s="22"/>
+      <c r="W307" s="22"/>
+    </row>
+    <row r="308" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="22"/>
+      <c r="B308" s="22"/>
+      <c r="C308" s="23"/>
+      <c r="D308" s="24">
+        <v>45617</v>
+      </c>
+      <c r="E308" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F308" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G308" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="H308" s="16">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I308" s="16">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="J308" s="22"/>
+      <c r="K308" s="22"/>
+      <c r="L308" s="22"/>
+      <c r="M308" s="22"/>
+      <c r="N308" s="22"/>
+      <c r="O308" s="22"/>
+      <c r="P308" s="22"/>
+      <c r="Q308" s="22"/>
+      <c r="R308" s="22"/>
+      <c r="S308" s="22"/>
+      <c r="T308" s="22"/>
+      <c r="U308" s="22"/>
+      <c r="V308" s="22"/>
+      <c r="W308" s="22"/>
+    </row>
+    <row r="309" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="22"/>
+      <c r="B309" s="22"/>
+      <c r="C309" s="23"/>
+      <c r="D309" s="24">
+        <v>45618</v>
+      </c>
+      <c r="E309" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F309" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G309" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H309" s="16">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="I309" s="16">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="J309" s="22"/>
+      <c r="K309" s="22"/>
+      <c r="L309" s="22"/>
+      <c r="M309" s="22"/>
+      <c r="N309" s="22"/>
+      <c r="O309" s="22"/>
+      <c r="P309" s="22"/>
+      <c r="Q309" s="22"/>
+      <c r="R309" s="22"/>
+      <c r="S309" s="22"/>
+      <c r="T309" s="22"/>
+      <c r="U309" s="22"/>
+      <c r="V309" s="22"/>
+      <c r="W309" s="22"/>
+    </row>
+    <row r="310" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="22"/>
+      <c r="B310" s="22"/>
+      <c r="C310" s="23"/>
+      <c r="D310" s="36">
+        <v>45618</v>
+      </c>
+      <c r="E310" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F310" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G310" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="H310" s="19">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I310" s="19">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="J310" s="22"/>
+      <c r="K310" s="22"/>
+      <c r="L310" s="22"/>
+      <c r="M310" s="22"/>
+      <c r="N310" s="22"/>
+      <c r="O310" s="22"/>
+      <c r="P310" s="22"/>
+      <c r="Q310" s="22"/>
+      <c r="R310" s="22"/>
+      <c r="S310" s="22"/>
+      <c r="T310" s="22"/>
+      <c r="U310" s="22"/>
+      <c r="V310" s="22"/>
+      <c r="W310" s="22"/>
+    </row>
+    <row r="311" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="22"/>
+      <c r="B311" s="22"/>
+      <c r="C311" s="23"/>
+      <c r="D311" s="24">
+        <v>45618</v>
+      </c>
+      <c r="E311" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F311" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G311" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="H311" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="I311" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="J311" s="22"/>
+      <c r="K311" s="22"/>
+      <c r="L311" s="22"/>
+      <c r="M311" s="22"/>
+      <c r="N311" s="22"/>
+    </row>
+    <row r="312" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="22"/>
+      <c r="B312" s="22"/>
+      <c r="C312" s="23"/>
+      <c r="D312" s="36">
+        <v>45618</v>
+      </c>
+      <c r="E312" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F312" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G312" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="H312" s="19">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I312" s="19">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="J312" s="22"/>
+      <c r="K312" s="22"/>
+      <c r="L312" s="22"/>
+      <c r="M312" s="22"/>
+      <c r="N312" s="22"/>
+    </row>
+    <row r="313" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D313" s="4">
+        <v>45618</v>
+      </c>
+      <c r="E313" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F313" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G313" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="H313" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I313" s="6">
+        <v>0.55902777777777779</v>
+      </c>
+    </row>
+    <row r="314" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D314" s="4">
+        <v>45621</v>
+      </c>
+      <c r="E314" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F314" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G314" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H314" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="I314" s="6">
+        <v>0.48958333333333331</v>
+      </c>
+    </row>
+    <row r="315" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D315" s="4">
+        <v>45622</v>
+      </c>
+      <c r="E315" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F315" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G315" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="H315" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="I315" s="6">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="316" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D316" s="4">
+        <v>45622</v>
+      </c>
+      <c r="E316" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F316" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G316" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="H316" s="6">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="I316" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="317" spans="1:23" s="52" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D317" s="4">
+        <v>45622</v>
+      </c>
+      <c r="E317" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F317" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G317" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H317" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="I317" s="6">
+        <v>0.47569444444444442</v>
+      </c>
+    </row>
+    <row r="318" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D318" s="4">
+        <v>45622</v>
+      </c>
+      <c r="E318" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F318" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G318" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H318" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I318" s="6">
+        <v>0.55625000000000002</v>
+      </c>
+    </row>
+    <row r="319" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D319" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E319" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F319" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G319" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H319" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I319" s="6">
+        <v>0.33680555555555558</v>
+      </c>
+    </row>
+    <row r="320" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D320" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E320" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F320" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G320" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="H320" s="6">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="I320" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="321" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D321" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E321" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F321" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G321" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H321" s="6">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="I321" s="6">
+        <v>0.35694444444444445</v>
+      </c>
+    </row>
+    <row r="322" spans="1:24" s="53" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D322" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E322" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F322" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G322" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="H322" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I322" s="6">
+        <v>0.42083333333333334</v>
+      </c>
+    </row>
+    <row r="323" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D323" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E323" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F323" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G323" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="H323" s="6">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="I323" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="324" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D324" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E324" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F324" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G324" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="H324" s="6">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="I324" s="6">
+        <v>0.47222222222222227</v>
+      </c>
+    </row>
+    <row r="325" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D325" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E325" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F325" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G325" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="H325" s="6">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="I325" s="6">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="326" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D326" s="4">
+        <v>45623</v>
+      </c>
+      <c r="E326" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F326" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G326" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="H326" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I326" s="6">
+        <v>0.52777777777777779</v>
+      </c>
+    </row>
+    <row r="327" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="22"/>
+      <c r="B327" s="22"/>
+      <c r="C327" s="23"/>
+      <c r="D327" s="24">
+        <v>45624</v>
+      </c>
+      <c r="E327" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F327" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G327" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="H327" s="16">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="I327" s="16">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="J327" s="22"/>
+      <c r="K327" s="22"/>
+      <c r="L327" s="22"/>
+      <c r="M327" s="22"/>
+      <c r="N327" s="22"/>
+      <c r="O327" s="22"/>
+      <c r="P327" s="22"/>
+      <c r="Q327" s="22"/>
+      <c r="R327" s="22"/>
+      <c r="S327" s="22"/>
+      <c r="T327" s="22"/>
+      <c r="U327" s="22"/>
+      <c r="V327" s="22"/>
+      <c r="W327" s="22"/>
+      <c r="X327" s="22"/>
+    </row>
+    <row r="328" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="22"/>
+      <c r="B328" s="22"/>
+      <c r="C328" s="23"/>
+      <c r="D328" s="36">
+        <v>45624</v>
+      </c>
+      <c r="E328" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F328" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G328" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="H328" s="19">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I328" s="19">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="J328" s="22"/>
+      <c r="K328" s="22"/>
+      <c r="L328" s="22"/>
+      <c r="M328" s="22"/>
+      <c r="N328" s="22"/>
+      <c r="O328" s="22"/>
+      <c r="P328" s="22"/>
+      <c r="Q328" s="22"/>
+      <c r="R328" s="22"/>
+      <c r="S328" s="22"/>
+      <c r="T328" s="22"/>
+      <c r="U328" s="22"/>
+      <c r="V328" s="22"/>
+      <c r="W328" s="22"/>
+      <c r="X328" s="22"/>
+    </row>
+    <row r="329" spans="1:24" s="59" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="55"/>
+      <c r="B329" s="55"/>
+      <c r="C329" s="56"/>
+      <c r="D329" s="57">
+        <v>45624</v>
+      </c>
+      <c r="E329" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F329" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G329" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="H329" s="54">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="I329" s="54">
+        <v>0.40625</v>
+      </c>
+      <c r="J329" s="55"/>
+      <c r="K329" s="55"/>
+      <c r="L329" s="55"/>
+      <c r="M329" s="55"/>
+      <c r="N329" s="55"/>
+      <c r="O329" s="55"/>
+      <c r="P329" s="55"/>
+      <c r="Q329" s="55"/>
+      <c r="R329" s="55"/>
+      <c r="S329" s="55"/>
+      <c r="T329" s="55"/>
+      <c r="U329" s="55"/>
+      <c r="V329" s="55"/>
+      <c r="W329" s="55"/>
+      <c r="X329" s="55"/>
+    </row>
+    <row r="330" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="22"/>
+      <c r="B330" s="22"/>
+      <c r="C330" s="23"/>
+      <c r="D330" s="36">
+        <v>45624</v>
+      </c>
+      <c r="E330" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F330" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G330" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H330" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I330" s="19">
+        <v>0.46875</v>
+      </c>
+      <c r="J330" s="22"/>
+      <c r="K330" s="22"/>
+      <c r="L330" s="22"/>
+      <c r="M330" s="22"/>
+      <c r="N330" s="22"/>
+      <c r="O330" s="22"/>
+      <c r="P330" s="22"/>
+      <c r="Q330" s="22"/>
+      <c r="R330" s="22"/>
+      <c r="S330" s="22"/>
+      <c r="T330" s="22"/>
+      <c r="U330" s="22"/>
+      <c r="V330" s="22"/>
+      <c r="W330" s="22"/>
+      <c r="X330" s="22"/>
+    </row>
+    <row r="331" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="22"/>
+      <c r="B331" s="22"/>
+      <c r="C331" s="23"/>
+      <c r="D331" s="36">
+        <v>45624</v>
+      </c>
+      <c r="E331" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F331" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G331" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="H331" s="19">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="I331" s="19">
+        <v>0.49791666666666662</v>
+      </c>
+      <c r="J331" s="22"/>
+      <c r="K331" s="22"/>
+      <c r="L331" s="22"/>
+      <c r="M331" s="22"/>
+      <c r="N331" s="22"/>
+      <c r="O331" s="22"/>
+      <c r="P331" s="22"/>
+      <c r="Q331" s="22"/>
+      <c r="R331" s="22"/>
+      <c r="S331" s="22"/>
+      <c r="T331" s="22"/>
+      <c r="U331" s="22"/>
+      <c r="V331" s="22"/>
+      <c r="W331" s="22"/>
+      <c r="X331" s="22"/>
+    </row>
+    <row r="332" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="22"/>
+      <c r="B332" s="22"/>
+      <c r="C332" s="23"/>
+      <c r="D332" s="24">
+        <v>45625</v>
+      </c>
+      <c r="E332" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F332" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G332" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="H332" s="16">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="I332" s="16">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="J332" s="22"/>
+      <c r="K332" s="22"/>
+      <c r="L332" s="22"/>
+      <c r="M332" s="22"/>
+      <c r="N332" s="22"/>
+      <c r="O332" s="22"/>
+      <c r="P332" s="22"/>
+      <c r="Q332" s="22"/>
+      <c r="R332" s="22"/>
+      <c r="S332" s="22"/>
+      <c r="T332" s="22"/>
+      <c r="U332" s="22"/>
+      <c r="V332" s="22"/>
+      <c r="W332" s="22"/>
+      <c r="X332" s="22"/>
+    </row>
+    <row r="333" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="22"/>
+      <c r="B333" s="22"/>
+      <c r="C333" s="23"/>
+      <c r="D333" s="36">
+        <v>45625</v>
+      </c>
+      <c r="E333" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F333" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G333" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="H333" s="19">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I333" s="19">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="J333" s="22"/>
+      <c r="K333" s="22"/>
+      <c r="L333" s="22"/>
+      <c r="M333" s="22"/>
+      <c r="N333" s="22"/>
+      <c r="O333" s="22"/>
+      <c r="P333" s="22"/>
+      <c r="Q333" s="22"/>
+      <c r="R333" s="22"/>
+      <c r="S333" s="22"/>
+      <c r="T333" s="22"/>
+      <c r="U333" s="22"/>
+      <c r="V333" s="22"/>
+      <c r="W333" s="22"/>
+      <c r="X333" s="22"/>
+    </row>
+    <row r="334" spans="1:24" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="22"/>
+      <c r="B334" s="22"/>
+      <c r="C334" s="23"/>
+      <c r="D334" s="57">
+        <v>45625</v>
+      </c>
+      <c r="E334" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F334" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G334" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="H334" s="54">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="I334" s="54">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J334" s="22"/>
+      <c r="K334" s="22"/>
+      <c r="L334" s="22"/>
+      <c r="M334" s="22"/>
+      <c r="N334" s="22"/>
+      <c r="O334" s="22"/>
+      <c r="P334" s="22"/>
+      <c r="Q334" s="22"/>
+      <c r="R334" s="22"/>
+      <c r="S334" s="22"/>
+      <c r="T334" s="22"/>
+      <c r="U334" s="22"/>
+      <c r="V334" s="22"/>
+      <c r="W334" s="22"/>
+      <c r="X334" s="22"/>
+    </row>
+    <row r="335" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="22"/>
+      <c r="B335" s="22"/>
+      <c r="C335" s="23"/>
+      <c r="D335" s="24">
+        <v>45628</v>
+      </c>
+      <c r="E335" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F335" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G335" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="H335" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I335" s="16">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="J335" s="22"/>
+      <c r="K335" s="22"/>
+      <c r="L335" s="22"/>
+      <c r="M335" s="22"/>
+      <c r="N335" s="22"/>
+      <c r="O335" s="22"/>
+      <c r="P335" s="22"/>
+      <c r="Q335" s="22"/>
+      <c r="R335" s="22"/>
+      <c r="S335" s="22"/>
+      <c r="T335" s="22"/>
+      <c r="U335" s="22"/>
+      <c r="V335" s="22"/>
+      <c r="W335" s="22"/>
+      <c r="X335" s="22"/>
+    </row>
+    <row r="336" spans="1:24" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="22"/>
+      <c r="B336" s="22"/>
+      <c r="C336" s="23"/>
+      <c r="D336" s="57">
+        <v>45628</v>
+      </c>
+      <c r="E336" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F336" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="G336" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="H336" s="54">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I336" s="54">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="J336" s="22"/>
+      <c r="K336" s="22"/>
+      <c r="L336" s="22"/>
+      <c r="M336" s="22"/>
+      <c r="N336" s="22"/>
+      <c r="O336" s="22"/>
+      <c r="P336" s="22"/>
+      <c r="Q336" s="22"/>
+      <c r="R336" s="22"/>
+      <c r="S336" s="22"/>
+      <c r="T336" s="22"/>
+      <c r="U336" s="22"/>
+      <c r="V336" s="22"/>
+      <c r="W336" s="22"/>
+      <c r="X336" s="22"/>
+    </row>
+    <row r="337" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="22"/>
+      <c r="B337" s="22"/>
+      <c r="C337" s="23"/>
+      <c r="D337" s="36">
+        <v>45628</v>
+      </c>
+      <c r="E337" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F337" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G337" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="H337" s="19">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="I337" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J337" s="22"/>
+      <c r="K337" s="22"/>
+      <c r="L337" s="22"/>
+      <c r="M337" s="22"/>
+      <c r="N337" s="22"/>
+      <c r="O337" s="22"/>
+      <c r="P337" s="22"/>
+      <c r="Q337" s="22"/>
+      <c r="R337" s="22"/>
+      <c r="S337" s="22"/>
+      <c r="T337" s="22"/>
+      <c r="U337" s="22"/>
+      <c r="V337" s="22"/>
+      <c r="W337" s="22"/>
+      <c r="X337" s="22"/>
+    </row>
+    <row r="338" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="22"/>
+      <c r="B338" s="22"/>
+      <c r="C338" s="23"/>
+      <c r="D338" s="36">
+        <v>45628</v>
+      </c>
+      <c r="E338" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F338" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G338" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="H338" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="I338" s="19">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="J338" s="22"/>
+      <c r="K338" s="22"/>
+      <c r="L338" s="22"/>
+      <c r="M338" s="22"/>
+      <c r="N338" s="22"/>
+      <c r="O338" s="22"/>
+      <c r="P338" s="22"/>
+      <c r="Q338" s="22"/>
+      <c r="R338" s="22"/>
+      <c r="S338" s="22"/>
+      <c r="T338" s="22"/>
+      <c r="U338" s="22"/>
+      <c r="V338" s="22"/>
+      <c r="W338" s="22"/>
+      <c r="X338" s="22"/>
+    </row>
+    <row r="339" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="22"/>
+      <c r="B339" s="22"/>
+      <c r="C339" s="23"/>
+      <c r="D339" s="36">
+        <v>45628</v>
+      </c>
+      <c r="E339" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F339" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G339" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="H339" s="19">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="I339" s="19">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="J339" s="22"/>
+      <c r="K339" s="22"/>
+      <c r="L339" s="22"/>
+      <c r="M339" s="22"/>
+      <c r="N339" s="22"/>
+      <c r="O339" s="22"/>
+      <c r="P339" s="22"/>
+      <c r="Q339" s="22"/>
+      <c r="R339" s="22"/>
+      <c r="S339" s="22"/>
+      <c r="T339" s="22"/>
+      <c r="U339" s="22"/>
+      <c r="V339" s="22"/>
+      <c r="W339" s="22"/>
+      <c r="X339" s="22"/>
+    </row>
+    <row r="340" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="22"/>
+      <c r="B340" s="22"/>
+      <c r="C340" s="23"/>
+      <c r="D340" s="24">
+        <v>45629</v>
+      </c>
+      <c r="E340" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F340" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G340" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="H340" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I340" s="16">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="J340" s="22"/>
+      <c r="K340" s="22"/>
+      <c r="L340" s="22"/>
+      <c r="M340" s="22"/>
+      <c r="N340" s="22"/>
+      <c r="O340" s="22"/>
+      <c r="P340" s="22"/>
+      <c r="Q340" s="22"/>
+      <c r="R340" s="22"/>
+      <c r="S340" s="22"/>
+      <c r="T340" s="22"/>
+      <c r="U340" s="22"/>
+      <c r="V340" s="22"/>
+      <c r="W340" s="22"/>
+      <c r="X340" s="22"/>
+    </row>
+    <row r="341" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="22"/>
+      <c r="B341" s="22"/>
+      <c r="C341" s="23"/>
+      <c r="D341" s="36">
+        <v>45629</v>
+      </c>
+      <c r="E341" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F341" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G341" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="H341" s="19">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="I341" s="19">
+        <v>0.34375</v>
+      </c>
+      <c r="J341" s="22"/>
+      <c r="K341" s="22"/>
+      <c r="L341" s="22"/>
+      <c r="M341" s="22"/>
+      <c r="N341" s="22"/>
+      <c r="O341" s="22"/>
+      <c r="P341" s="22"/>
+      <c r="Q341" s="22"/>
+      <c r="R341" s="22"/>
+      <c r="S341" s="22"/>
+      <c r="T341" s="22"/>
+      <c r="U341" s="22"/>
+      <c r="V341" s="22"/>
+      <c r="W341" s="22"/>
+      <c r="X341" s="22"/>
+    </row>
+    <row r="342" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="22"/>
+      <c r="B342" s="22"/>
+      <c r="C342" s="23"/>
+      <c r="D342" s="36">
+        <v>45629</v>
+      </c>
+      <c r="E342" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F342" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G342" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="H342" s="19">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="I342" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J342" s="22"/>
+      <c r="K342" s="22"/>
+      <c r="L342" s="22"/>
+      <c r="M342" s="22"/>
+      <c r="N342" s="22"/>
+      <c r="O342" s="22"/>
+      <c r="P342" s="22"/>
+      <c r="Q342" s="22"/>
+      <c r="R342" s="22"/>
+      <c r="S342" s="22"/>
+      <c r="T342" s="22"/>
+      <c r="U342" s="22"/>
+      <c r="V342" s="22"/>
+      <c r="W342" s="22"/>
+      <c r="X342" s="22"/>
+    </row>
+    <row r="343" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="22"/>
+      <c r="B343" s="22"/>
+      <c r="C343" s="23"/>
+      <c r="D343" s="36">
+        <v>45629</v>
+      </c>
+      <c r="E343" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F343" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G343" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="H343" s="19">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="I343" s="19">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="J343" s="22"/>
+      <c r="K343" s="22"/>
+      <c r="L343" s="22"/>
+      <c r="M343" s="22"/>
+      <c r="N343" s="22"/>
+      <c r="O343" s="22"/>
+      <c r="P343" s="22"/>
+      <c r="Q343" s="22"/>
+      <c r="R343" s="22"/>
+      <c r="S343" s="22"/>
+      <c r="T343" s="22"/>
+      <c r="U343" s="22"/>
+      <c r="V343" s="22"/>
+      <c r="W343" s="22"/>
+      <c r="X343" s="22"/>
+    </row>
+    <row r="344" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="22"/>
+      <c r="B344" s="22"/>
+      <c r="C344" s="23"/>
+      <c r="D344" s="24">
+        <v>45630</v>
+      </c>
+      <c r="E344" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F344" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G344" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="H344" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I344" s="16">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="J344" s="22"/>
+      <c r="K344" s="22"/>
+      <c r="L344" s="22"/>
+      <c r="M344" s="22"/>
+      <c r="N344" s="22"/>
+      <c r="O344" s="22"/>
+      <c r="P344" s="22"/>
+      <c r="Q344" s="22"/>
+      <c r="R344" s="22"/>
+      <c r="S344" s="22"/>
+      <c r="T344" s="22"/>
+      <c r="U344" s="22"/>
+      <c r="V344" s="22"/>
+      <c r="W344" s="22"/>
+      <c r="X344" s="22"/>
+    </row>
+    <row r="345" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="22"/>
+      <c r="B345" s="22"/>
+      <c r="C345" s="23"/>
+      <c r="D345" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E345" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F345" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G345" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="H345" s="19">
+        <v>0.34375</v>
+      </c>
+      <c r="I345" s="19">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="J345" s="22"/>
+      <c r="K345" s="22"/>
+      <c r="L345" s="22"/>
+      <c r="M345" s="22"/>
+      <c r="N345" s="22"/>
+      <c r="O345" s="22"/>
+      <c r="P345" s="22"/>
+      <c r="Q345" s="22"/>
+      <c r="R345" s="22"/>
+      <c r="S345" s="22"/>
+      <c r="T345" s="22"/>
+      <c r="U345" s="22"/>
+      <c r="V345" s="22"/>
+      <c r="W345" s="22"/>
+      <c r="X345" s="22"/>
+    </row>
+    <row r="346" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="22"/>
+      <c r="B346" s="22"/>
+      <c r="C346" s="23"/>
+      <c r="D346" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E346" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F346" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G346" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="H346" s="19">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I346" s="19">
+        <v>0.375</v>
+      </c>
+      <c r="J346" s="22"/>
+      <c r="K346" s="22"/>
+      <c r="L346" s="22"/>
+      <c r="M346" s="22"/>
+      <c r="N346" s="22"/>
+      <c r="O346" s="22"/>
+      <c r="P346" s="22"/>
+      <c r="Q346" s="22"/>
+      <c r="R346" s="22"/>
+      <c r="S346" s="22"/>
+      <c r="T346" s="22"/>
+      <c r="U346" s="22"/>
+      <c r="V346" s="22"/>
+      <c r="W346" s="22"/>
+      <c r="X346" s="22"/>
+    </row>
+    <row r="347" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="22"/>
+      <c r="B347" s="22"/>
+      <c r="C347" s="23"/>
+      <c r="D347" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E347" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F347" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G347" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="H347" s="19">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="I347" s="19">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="J347" s="22"/>
+      <c r="K347" s="22"/>
+      <c r="L347" s="22"/>
+      <c r="M347" s="22"/>
+      <c r="N347" s="22"/>
+      <c r="O347" s="22"/>
+      <c r="P347" s="22"/>
+      <c r="Q347" s="22"/>
+      <c r="R347" s="22"/>
+      <c r="S347" s="22"/>
+      <c r="T347" s="22"/>
+      <c r="U347" s="22"/>
+      <c r="V347" s="22"/>
+      <c r="W347" s="22"/>
+      <c r="X347" s="22"/>
+    </row>
+    <row r="348" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="22"/>
+      <c r="B348" s="22"/>
+      <c r="C348" s="23"/>
+      <c r="D348" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E348" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F348" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G348" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="H348" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I348" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J348" s="22"/>
+      <c r="K348" s="22"/>
+      <c r="L348" s="22"/>
+      <c r="M348" s="22"/>
+      <c r="N348" s="22"/>
+      <c r="O348" s="22"/>
+      <c r="P348" s="22"/>
+      <c r="Q348" s="22"/>
+      <c r="R348" s="22"/>
+      <c r="S348" s="22"/>
+      <c r="T348" s="22"/>
+      <c r="U348" s="22"/>
+      <c r="V348" s="22"/>
+      <c r="W348" s="22"/>
+      <c r="X348" s="22"/>
+    </row>
+    <row r="349" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="22"/>
+      <c r="B349" s="22"/>
+      <c r="C349" s="23"/>
+      <c r="D349" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E349" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F349" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G349" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="H349" s="19">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="I349" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="J349" s="22"/>
+      <c r="K349" s="22"/>
+      <c r="L349" s="22"/>
+      <c r="M349" s="22"/>
+      <c r="N349" s="22"/>
+      <c r="O349" s="22"/>
+      <c r="P349" s="22"/>
+      <c r="Q349" s="22"/>
+      <c r="R349" s="22"/>
+      <c r="S349" s="22"/>
+      <c r="T349" s="22"/>
+      <c r="U349" s="22"/>
+      <c r="V349" s="22"/>
+      <c r="W349" s="22"/>
+      <c r="X349" s="22"/>
+    </row>
+    <row r="350" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="22"/>
+      <c r="B350" s="22"/>
+      <c r="C350" s="23"/>
+      <c r="D350" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E350" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F350" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G350" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="H350" s="19">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I350" s="19">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="J350" s="22"/>
+      <c r="K350" s="22"/>
+      <c r="L350" s="22"/>
+      <c r="M350" s="22"/>
+      <c r="N350" s="22"/>
+      <c r="O350" s="22"/>
+      <c r="P350" s="22"/>
+      <c r="Q350" s="22"/>
+      <c r="R350" s="22"/>
+      <c r="S350" s="22"/>
+      <c r="T350" s="22"/>
+      <c r="U350" s="22"/>
+      <c r="V350" s="22"/>
+      <c r="W350" s="22"/>
+      <c r="X350" s="22"/>
+    </row>
+    <row r="351" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="22"/>
+      <c r="B351" s="22"/>
+      <c r="C351" s="23"/>
+      <c r="D351" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E351" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F351" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G351" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="H351" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I351" s="19">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="J351" s="22"/>
+      <c r="K351" s="22"/>
+      <c r="L351" s="22"/>
+      <c r="M351" s="22"/>
+      <c r="N351" s="22"/>
+      <c r="O351" s="22"/>
+      <c r="P351" s="22"/>
+      <c r="Q351" s="22"/>
+      <c r="R351" s="22"/>
+      <c r="S351" s="22"/>
+      <c r="T351" s="22"/>
+      <c r="U351" s="22"/>
+      <c r="V351" s="22"/>
+      <c r="W351" s="22"/>
+      <c r="X351" s="22"/>
+    </row>
+    <row r="352" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="22"/>
+      <c r="B352" s="22"/>
+      <c r="C352" s="23"/>
+      <c r="D352" s="36">
+        <v>45630</v>
+      </c>
+      <c r="E352" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F352" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G352" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="H352" s="19">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="I352" s="19">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="J352" s="22"/>
+      <c r="K352" s="22"/>
+      <c r="L352" s="22"/>
+      <c r="M352" s="22"/>
+      <c r="N352" s="22"/>
+      <c r="O352" s="22"/>
+      <c r="P352" s="22"/>
+      <c r="Q352" s="22"/>
+      <c r="R352" s="22"/>
+      <c r="S352" s="22"/>
+      <c r="T352" s="22"/>
+      <c r="U352" s="22"/>
+      <c r="V352" s="22"/>
+      <c r="W352" s="22"/>
+      <c r="X352" s="22"/>
+    </row>
+    <row r="353" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="22"/>
+      <c r="B353" s="22"/>
+      <c r="C353" s="23"/>
+      <c r="D353" s="24">
+        <v>45631</v>
+      </c>
+      <c r="E353" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F353" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G353" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="H353" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I353" s="16">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="J353" s="22"/>
+      <c r="K353" s="22"/>
+      <c r="L353" s="22"/>
+      <c r="M353" s="22"/>
+      <c r="N353" s="22"/>
+      <c r="O353" s="22"/>
+      <c r="P353" s="22"/>
+      <c r="Q353" s="22"/>
+      <c r="R353" s="22"/>
+      <c r="S353" s="22"/>
+      <c r="T353" s="22"/>
+      <c r="U353" s="22"/>
+      <c r="V353" s="22"/>
+      <c r="W353" s="22"/>
+      <c r="X353" s="22"/>
+    </row>
+    <row r="354" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="22"/>
+      <c r="B354" s="22"/>
+      <c r="C354" s="23"/>
+      <c r="D354" s="36">
+        <v>45631</v>
+      </c>
+      <c r="E354" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F354" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G354" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="H354" s="19">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I354" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="J354" s="22"/>
+      <c r="K354" s="22"/>
+      <c r="L354" s="22"/>
+      <c r="M354" s="22"/>
+      <c r="N354" s="22"/>
+      <c r="O354" s="22"/>
+      <c r="P354" s="22"/>
+      <c r="Q354" s="22"/>
+      <c r="R354" s="22"/>
+      <c r="S354" s="22"/>
+      <c r="T354" s="22"/>
+      <c r="U354" s="22"/>
+      <c r="V354" s="22"/>
+      <c r="W354" s="22"/>
+      <c r="X354" s="22"/>
+    </row>
+    <row r="355" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="22"/>
+      <c r="B355" s="22"/>
+      <c r="C355" s="23"/>
+      <c r="D355" s="36">
+        <v>45631</v>
+      </c>
+      <c r="E355" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F355" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G355" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="H355" s="19">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="I355" s="19">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="J355" s="22"/>
+      <c r="K355" s="22"/>
+      <c r="L355" s="22"/>
+      <c r="M355" s="22"/>
+      <c r="N355" s="22"/>
+      <c r="O355" s="22"/>
+      <c r="P355" s="22"/>
+      <c r="Q355" s="22"/>
+      <c r="R355" s="22"/>
+      <c r="S355" s="22"/>
+      <c r="T355" s="22"/>
+      <c r="U355" s="22"/>
+      <c r="V355" s="22"/>
+      <c r="W355" s="22"/>
+      <c r="X355" s="22"/>
+    </row>
+    <row r="356" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="22"/>
+      <c r="B356" s="22"/>
+      <c r="C356" s="23"/>
+      <c r="D356" s="36">
+        <v>45631</v>
+      </c>
+      <c r="E356" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F356" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G356" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="H356" s="19">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I356" s="19">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="J356" s="22"/>
+      <c r="K356" s="22"/>
+      <c r="L356" s="22"/>
+      <c r="M356" s="22"/>
+      <c r="N356" s="22"/>
+      <c r="O356" s="22"/>
+      <c r="P356" s="22"/>
+      <c r="Q356" s="22"/>
+      <c r="R356" s="22"/>
+      <c r="S356" s="22"/>
+      <c r="T356" s="22"/>
+      <c r="U356" s="22"/>
+      <c r="V356" s="22"/>
+      <c r="W356" s="22"/>
+      <c r="X356" s="22"/>
+    </row>
+    <row r="357" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D357" s="11"/>
       <c r="E357" s="10"/>
       <c r="F357" s="10"/>
@@ -8587,7 +10105,7 @@
       <c r="H357" s="11"/>
       <c r="I357" s="11"/>
     </row>
-    <row r="358" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D358" s="11"/>
       <c r="E358" s="10"/>
       <c r="F358" s="10"/>
@@ -8595,7 +10113,7 @@
       <c r="H358" s="11"/>
       <c r="I358" s="11"/>
     </row>
-    <row r="359" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D359" s="11"/>
       <c r="E359" s="10"/>
       <c r="F359" s="10"/>
@@ -8603,7 +10121,7 @@
       <c r="H359" s="11"/>
       <c r="I359" s="11"/>
     </row>
-    <row r="360" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D360" s="11"/>
       <c r="E360" s="10"/>
       <c r="F360" s="10"/>
@@ -8611,7 +10129,7 @@
       <c r="H360" s="11"/>
       <c r="I360" s="11"/>
     </row>
-    <row r="361" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D361" s="11"/>
       <c r="E361" s="10"/>
       <c r="F361" s="10"/>
@@ -8619,7 +10137,7 @@
       <c r="H361" s="11"/>
       <c r="I361" s="11"/>
     </row>
-    <row r="362" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D362" s="11"/>
       <c r="E362" s="10"/>
       <c r="F362" s="10"/>
@@ -8627,7 +10145,7 @@
       <c r="H362" s="11"/>
       <c r="I362" s="11"/>
     </row>
-    <row r="363" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D363" s="11"/>
       <c r="E363" s="10"/>
       <c r="F363" s="10"/>
@@ -8635,7 +10153,7 @@
       <c r="H363" s="11"/>
       <c r="I363" s="11"/>
     </row>
-    <row r="364" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D364" s="11"/>
       <c r="E364" s="10"/>
       <c r="F364" s="10"/>
@@ -8643,7 +10161,7 @@
       <c r="H364" s="11"/>
       <c r="I364" s="11"/>
     </row>
-    <row r="365" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D365" s="11"/>
       <c r="E365" s="10"/>
       <c r="F365" s="10"/>
@@ -8651,7 +10169,7 @@
       <c r="H365" s="11"/>
       <c r="I365" s="11"/>
     </row>
-    <row r="366" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D366" s="11"/>
       <c r="E366" s="10"/>
       <c r="F366" s="10"/>
@@ -8659,7 +10177,7 @@
       <c r="H366" s="11"/>
       <c r="I366" s="11"/>
     </row>
-    <row r="367" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D367" s="11"/>
       <c r="E367" s="10"/>
       <c r="F367" s="10"/>
@@ -8667,7 +10185,7 @@
       <c r="H367" s="11"/>
       <c r="I367" s="11"/>
     </row>
-    <row r="368" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D368" s="11"/>
       <c r="E368" s="10"/>
       <c r="F368" s="10"/>
@@ -13795,19 +15313,43 @@
       <c r="H1008" s="11"/>
       <c r="I1008" s="11"/>
     </row>
+    <row r="1009" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1009" s="11"/>
+      <c r="E1009" s="10"/>
+      <c r="F1009" s="10"/>
+      <c r="G1009" s="10"/>
+      <c r="H1009" s="11"/>
+      <c r="I1009" s="11"/>
+    </row>
+    <row r="1010" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1010" s="11"/>
+      <c r="E1010" s="10"/>
+      <c r="F1010" s="10"/>
+      <c r="G1010" s="10"/>
+      <c r="H1010" s="11"/>
+      <c r="I1010" s="11"/>
+    </row>
+    <row r="1011" spans="4:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1011" s="11"/>
+      <c r="E1011" s="10"/>
+      <c r="F1011" s="10"/>
+      <c r="G1011" s="10"/>
+      <c r="H1011" s="11"/>
+      <c r="I1011" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E282 E300:E1008">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E282 E300 E303:E306 E313:E326 E357:E1011">
       <formula1>"GABRIEL,UILLIAM"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F32 F40">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F282 F300:F1008">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F282 F300 F303:F306 F313:F326 F357:F1011">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CPA,CORD,BLIB,DIR,FIN,RH"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F28">

</xml_diff>

<commit_message>
📝 Atualizando dados da planilha
</commit_message>
<xml_diff>
--- a/Registro-de-atividades.xlsx
+++ b/Registro-de-atividades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="520">
   <si>
     <t>Registro de atividades</t>
   </si>
@@ -1564,6 +1564,21 @@
   </si>
   <si>
     <t>trocando ssd e processador do pc da clinica de odonto</t>
+  </si>
+  <si>
+    <t>Inslatando ssd no pc clinica de odonto</t>
+  </si>
+  <si>
+    <t>Baixando o ventoy para colocar no hd</t>
+  </si>
+  <si>
+    <t>Instalando pc para o mac na antiga sala do rh</t>
+  </si>
+  <si>
+    <t>Criando HD butavel</t>
+  </si>
+  <si>
+    <t>Instalando pc de Cilene na sala de Milena</t>
   </si>
 </sst>
 </file>
@@ -2359,7 +2374,7 @@
   <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
-      <selection activeCell="E573" sqref="E573"/>
+      <selection activeCell="D575" sqref="D575"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18887,45 +18902,200 @@
       <c r="X569" s="67"/>
       <c r="Y569" s="67"/>
     </row>
-    <row r="570" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D570" s="11"/>
-      <c r="E570" s="10"/>
-      <c r="F570" s="10"/>
-      <c r="G570" s="10"/>
-      <c r="H570" s="11"/>
-      <c r="I570" s="11"/>
-    </row>
-    <row r="571" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D571" s="11"/>
-      <c r="E571" s="10"/>
-      <c r="F571" s="10"/>
-      <c r="G571" s="10"/>
-      <c r="H571" s="11"/>
-      <c r="I571" s="11"/>
-    </row>
-    <row r="572" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D572" s="11"/>
-      <c r="E572" s="10"/>
-      <c r="F572" s="10"/>
-      <c r="G572" s="10"/>
-      <c r="H572" s="11"/>
-      <c r="I572" s="11"/>
-    </row>
-    <row r="573" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D573" s="11"/>
-      <c r="E573" s="10"/>
-      <c r="F573" s="10"/>
-      <c r="G573" s="10"/>
-      <c r="H573" s="11"/>
-      <c r="I573" s="11"/>
-    </row>
-    <row r="574" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D574" s="11"/>
-      <c r="E574" s="10"/>
-      <c r="F574" s="10"/>
-      <c r="G574" s="10"/>
-      <c r="H574" s="11"/>
-      <c r="I574" s="11"/>
+    <row r="570" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A570" s="69"/>
+      <c r="B570" s="70"/>
+      <c r="C570" s="66"/>
+      <c r="D570" s="24">
+        <v>45694</v>
+      </c>
+      <c r="E570" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F570" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G570" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="H570" s="16">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="I570" s="16">
+        <v>0.40625</v>
+      </c>
+      <c r="J570" s="66"/>
+      <c r="K570" s="71"/>
+      <c r="L570" s="72"/>
+      <c r="M570" s="66"/>
+      <c r="N570" s="66"/>
+      <c r="O570" s="66"/>
+      <c r="P570" s="66"/>
+      <c r="Q570" s="66"/>
+      <c r="R570" s="66"/>
+      <c r="S570" s="66"/>
+      <c r="T570" s="66"/>
+      <c r="U570" s="66"/>
+      <c r="V570" s="66"/>
+      <c r="W570" s="66"/>
+      <c r="X570" s="66"/>
+      <c r="Y570" s="66"/>
+    </row>
+    <row r="571" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A571" s="68"/>
+      <c r="B571" s="67"/>
+      <c r="C571" s="67"/>
+      <c r="D571" s="36">
+        <v>45694</v>
+      </c>
+      <c r="E571" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F571" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G571" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="H571" s="19">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="I571" s="19">
+        <v>0.46458333333333335</v>
+      </c>
+      <c r="J571" s="67"/>
+      <c r="K571" s="67"/>
+      <c r="L571" s="67"/>
+      <c r="M571" s="67"/>
+      <c r="N571" s="67"/>
+      <c r="O571" s="67"/>
+      <c r="P571" s="67"/>
+      <c r="Q571" s="67"/>
+      <c r="R571" s="67"/>
+      <c r="S571" s="67"/>
+      <c r="T571" s="67"/>
+      <c r="U571" s="67"/>
+      <c r="V571" s="67"/>
+      <c r="W571" s="67"/>
+      <c r="X571" s="67"/>
+      <c r="Y571" s="67"/>
+    </row>
+    <row r="572" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A572" s="69"/>
+      <c r="B572" s="70"/>
+      <c r="C572" s="67"/>
+      <c r="D572" s="36">
+        <v>45694</v>
+      </c>
+      <c r="E572" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F572" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G572" s="18" t="s">
+        <v>517</v>
+      </c>
+      <c r="H572" s="19">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="I572" s="19">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="J572" s="67"/>
+      <c r="K572" s="71"/>
+      <c r="L572" s="72"/>
+      <c r="M572" s="67"/>
+      <c r="N572" s="67"/>
+      <c r="O572" s="67"/>
+      <c r="P572" s="67"/>
+      <c r="Q572" s="67"/>
+      <c r="R572" s="67"/>
+      <c r="S572" s="67"/>
+      <c r="T572" s="67"/>
+      <c r="U572" s="67"/>
+      <c r="V572" s="67"/>
+      <c r="W572" s="67"/>
+      <c r="X572" s="67"/>
+      <c r="Y572" s="67"/>
+    </row>
+    <row r="573" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A573" s="69"/>
+      <c r="B573" s="70"/>
+      <c r="C573" s="67"/>
+      <c r="D573" s="36">
+        <v>45694</v>
+      </c>
+      <c r="E573" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F573" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G573" s="18" t="s">
+        <v>518</v>
+      </c>
+      <c r="H573" s="19">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I573" s="19">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="J573" s="67"/>
+      <c r="K573" s="71"/>
+      <c r="L573" s="72"/>
+      <c r="M573" s="67"/>
+      <c r="N573" s="67"/>
+      <c r="O573" s="67"/>
+      <c r="P573" s="67"/>
+      <c r="Q573" s="67"/>
+      <c r="R573" s="67"/>
+      <c r="S573" s="67"/>
+      <c r="T573" s="67"/>
+      <c r="U573" s="67"/>
+      <c r="V573" s="67"/>
+      <c r="W573" s="67"/>
+      <c r="X573" s="67"/>
+      <c r="Y573" s="67"/>
+    </row>
+    <row r="574" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A574" s="69"/>
+      <c r="B574" s="70"/>
+      <c r="C574" s="66"/>
+      <c r="D574" s="24">
+        <v>45694</v>
+      </c>
+      <c r="E574" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F574" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G574" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="H574" s="16">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="I574" s="16">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="J574" s="66"/>
+      <c r="K574" s="71"/>
+      <c r="L574" s="72"/>
+      <c r="M574" s="66"/>
+      <c r="N574" s="66"/>
+      <c r="O574" s="66"/>
+      <c r="P574" s="66"/>
+      <c r="Q574" s="66"/>
+      <c r="R574" s="66"/>
+      <c r="S574" s="66"/>
+      <c r="T574" s="66"/>
+      <c r="U574" s="66"/>
+      <c r="V574" s="66"/>
+      <c r="W574" s="66"/>
+      <c r="X574" s="66"/>
+      <c r="Y574" s="66"/>
     </row>
     <row r="575" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D575" s="11"/>
@@ -22424,17 +22594,11 @@
       <c r="I1011" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="262">
-    <mergeCell ref="A564:B564"/>
-    <mergeCell ref="K564:L564"/>
-    <mergeCell ref="A566:B566"/>
-    <mergeCell ref="K566:L566"/>
-    <mergeCell ref="A567:B567"/>
-    <mergeCell ref="K567:L567"/>
-    <mergeCell ref="A568:B568"/>
-    <mergeCell ref="K568:L568"/>
-    <mergeCell ref="A569:B569"/>
-    <mergeCell ref="K569:L569"/>
+  <mergeCells count="270">
+    <mergeCell ref="A565:B565"/>
+    <mergeCell ref="K565:L565"/>
+    <mergeCell ref="A574:B574"/>
+    <mergeCell ref="K574:L574"/>
     <mergeCell ref="A551:B551"/>
     <mergeCell ref="K551:L551"/>
     <mergeCell ref="A530:B530"/>
@@ -22663,8 +22827,6 @@
     <mergeCell ref="K546:L546"/>
     <mergeCell ref="A547:B547"/>
     <mergeCell ref="K547:L547"/>
-    <mergeCell ref="A565:B565"/>
-    <mergeCell ref="K565:L565"/>
     <mergeCell ref="A557:B557"/>
     <mergeCell ref="K557:L557"/>
     <mergeCell ref="A558:B558"/>
@@ -22679,6 +22841,10 @@
     <mergeCell ref="K555:L555"/>
     <mergeCell ref="A556:B556"/>
     <mergeCell ref="K556:L556"/>
+    <mergeCell ref="A572:B572"/>
+    <mergeCell ref="K572:L572"/>
+    <mergeCell ref="A573:B573"/>
+    <mergeCell ref="K573:L573"/>
     <mergeCell ref="A559:B559"/>
     <mergeCell ref="K559:L559"/>
     <mergeCell ref="A560:B560"/>
@@ -22687,15 +22853,27 @@
     <mergeCell ref="K561:L561"/>
     <mergeCell ref="A562:B562"/>
     <mergeCell ref="K562:L562"/>
+    <mergeCell ref="A570:B570"/>
+    <mergeCell ref="K570:L570"/>
+    <mergeCell ref="A564:B564"/>
+    <mergeCell ref="K564:L564"/>
+    <mergeCell ref="A566:B566"/>
+    <mergeCell ref="K566:L566"/>
+    <mergeCell ref="A567:B567"/>
+    <mergeCell ref="K567:L567"/>
+    <mergeCell ref="A568:B568"/>
+    <mergeCell ref="K568:L568"/>
+    <mergeCell ref="A569:B569"/>
+    <mergeCell ref="K569:L569"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E282 E300 E303:E306 E313:E326 E403 E414:E415 E570:E1011">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E176 E180:E183 E188:E194 E196 E202:E203 E207:E208 E239:E243 E254:E257 E267:E278 E280:E282 E300 E303:E306 E313:E326 E403 E414:E415 E575:E1011">
       <formula1>"GABRIEL,UILLIAM"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F32 F40">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F282 F300 F303:F306 F313:F326 F403 F414:F415 F570:F1011">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F27 F29:F31 F33:F39 F41:F176 F180:F183 F188:F194 F196 F202:F203 F207:F208 F239:F243 F254:F257 F267:F278 F280:F282 F300 F303:F306 F313:F326 F403 F414:F415 F575:F1011">
       <formula1>"TI,NPJ,LAB,MED,PAV01,EAD,AULA,CORD MED,PROF MED,PROG,ARQ,ATEND,CAP,CPA,CORD,BLIB,DIR,FIN,RH"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F28">

</xml_diff>